<commit_message>
bug fix : import previsionnel tableau de bord
</commit_message>
<xml_diff>
--- a/web/files/compta/tableau_bord/fichier_import_tableau_bord_previsionnel.xlsx
+++ b/web/files/compta/tableau_bord/fichier_import_tableau_bord_previsionnel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\jaimeGerer\web\files\compta\tableau_bord\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1299279-0C05-46AB-BA4F-58FE548C4B9C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="28515" windowHeight="12075"/>
+    <workbookView xWindow="3528" yWindow="1392" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>Janvier</t>
   </si>
@@ -157,12 +163,18 @@
   </si>
   <si>
     <t>Web public</t>
+  </si>
+  <si>
+    <t>Frais refacturables public</t>
+  </si>
+  <si>
+    <t>Frais refacturables privé</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
@@ -249,6 +261,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -296,7 +311,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -329,9 +344,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,6 +396,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -539,21 +588,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" style="1" customWidth="1"/>
-    <col min="2" max="13" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="39.5546875" style="1" customWidth="1"/>
+    <col min="2" max="13" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -594,7 +643,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -613,7 +662,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
@@ -632,7 +681,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
@@ -651,7 +700,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
@@ -670,7 +719,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
@@ -689,7 +738,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
@@ -708,7 +757,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
@@ -727,7 +776,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>42</v>
       </c>
@@ -746,7 +795,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>41</v>
       </c>
@@ -765,7 +814,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
@@ -784,7 +833,7 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
@@ -803,7 +852,7 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>45</v>
       </c>
@@ -822,7 +871,7 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
@@ -841,7 +890,7 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -860,7 +909,7 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>35</v>
       </c>
@@ -879,7 +928,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
@@ -898,7 +947,7 @@
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
@@ -917,7 +966,7 @@
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
@@ -936,7 +985,7 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
@@ -955,7 +1004,7 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
@@ -974,7 +1023,7 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>42</v>
       </c>
@@ -993,7 +1042,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>41</v>
       </c>
@@ -1012,7 +1061,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
@@ -1031,7 +1080,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>44</v>
       </c>
@@ -1050,7 +1099,7 @@
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>45</v>
       </c>
@@ -1069,7 +1118,7 @@
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>46</v>
       </c>
@@ -1088,28 +1137,28 @@
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1126,28 +1175,28 @@
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1164,28 +1213,28 @@
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1202,28 +1251,28 @@
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
+    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1240,9 +1289,9 @@
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1259,9 +1308,9 @@
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1278,9 +1327,9 @@
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
     </row>
-    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1297,9 +1346,9 @@
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
     </row>
-    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1316,9 +1365,9 @@
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
     </row>
-    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1335,9 +1384,9 @@
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
     </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1354,9 +1403,9 @@
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
     </row>
-    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1373,9 +1422,9 @@
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
     </row>
-    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1392,9 +1441,9 @@
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
     </row>
-    <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1411,9 +1460,9 @@
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
     </row>
-    <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1430,9 +1479,9 @@
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
     </row>
-    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1449,9 +1498,9 @@
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
     </row>
-    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1468,27 +1517,29 @@
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
     </row>
-    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
+    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
     </row>
-    <row r="49" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
+    <row r="49" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1504,24 +1555,26 @@
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
+    <row r="50" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1538,7 +1591,7 @@
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1555,6 +1608,40 @@
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
     </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
@@ -1562,24 +1649,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>